<commit_message>
separar y juntar texto
</commit_message>
<xml_diff>
--- a/orders_has_products.xlsx
+++ b/orders_has_products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Excel-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{308C4F1A-C5CF-4B09-899D-7A48A1EACA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E04040FC-30CE-4956-AC13-25CD3735BFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="90">
   <si>
     <t>order_id</t>
   </si>
@@ -55,9 +55,6 @@
     <t>delivery_date</t>
   </si>
   <si>
-    <t xml:space="preserve">ship_name </t>
-  </si>
-  <si>
     <t xml:space="preserve">ship_address </t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t xml:space="preserve">Apple </t>
   </si>
   <si>
-    <t>Anna Addison</t>
-  </si>
-  <si>
     <t>1325 Candy Rd, San Francisco, CA 96123</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t xml:space="preserve"> Microsoft </t>
   </si>
   <si>
-    <t>Carol Campbell</t>
-  </si>
-  <si>
     <t>1931 Brown St, Gainesville, FL 85321</t>
   </si>
   <si>
@@ -115,9 +106,6 @@
     <t>Iphone 8</t>
   </si>
   <si>
-    <t xml:space="preserve">Julia Jones </t>
-  </si>
-  <si>
     <t xml:space="preserve">1622 Seaside St, Seattle, WA 32569 </t>
   </si>
   <si>
@@ -133,9 +121,6 @@
     <t>Ipad Mini 3th gen</t>
   </si>
   <si>
-    <t xml:space="preserve">Irene Everly </t>
-  </si>
-  <si>
     <t>1756 East Dr, Houston, TX 28562</t>
   </si>
   <si>
@@ -151,9 +136,6 @@
     <t>ESC8000 G4</t>
   </si>
   <si>
-    <t>Rachel Rose</t>
-  </si>
-  <si>
     <t xml:space="preserve">1465 River Dr, Boston, MA 43625 </t>
   </si>
   <si>
@@ -175,9 +157,6 @@
     <t xml:space="preserve">Monoprice </t>
   </si>
   <si>
-    <t>Sophie Sutton</t>
-  </si>
-  <si>
     <t>1896 West Dr, Portland, OR 65842</t>
   </si>
   <si>
@@ -187,9 +166,6 @@
     <t>Monoprice Ultra Slim Series High Speed HDMI Cable - 4K</t>
   </si>
   <si>
-    <t>Wendy West</t>
-  </si>
-  <si>
     <t>1252 Vine St, Chicago, IL 73215</t>
   </si>
   <si>
@@ -242,6 +218,84 @@
   </si>
   <si>
     <t>Reclamo</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>ship_name</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Addison</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>Campbell</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Everly</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Sutton</t>
+  </si>
+  <si>
+    <t>Wendy</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Concatenado</t>
+  </si>
+  <si>
+    <t>10 Addison 1000</t>
+  </si>
+  <si>
+    <t>10 Campbell 1001</t>
+  </si>
+  <si>
+    <t>10 Jones 1002</t>
+  </si>
+  <si>
+    <t>10 Everly 1003</t>
+  </si>
+  <si>
+    <t>10 Rose 1004</t>
+  </si>
+  <si>
+    <t>10 Sutton 1005</t>
+  </si>
+  <si>
+    <t>10 West 1006</t>
+  </si>
+  <si>
+    <t>Order_extraer</t>
   </si>
 </sst>
 </file>
@@ -749,7 +803,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -758,6 +812,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1117,12 +1172,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomLeft" activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,14 +1194,17 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="7"/>
+    <col min="13" max="13" width="13.28515625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.42578125" customWidth="1"/>
+    <col min="18" max="18" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1154,13 +1212,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1183,32 +1241,44 @@
       <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -1216,13 +1286,13 @@
         <v>1200</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>5000</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1201</v>
@@ -1245,33 +1315,50 @@
       <c r="L2" s="5">
         <v>43393</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="7">
+        <f>MONTH(L2)</f>
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>1000</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2">
+      <c r="T2" t="str">
+        <f>LEFT(S2,2)</f>
+        <v>ZW</v>
+      </c>
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="Q2">
-        <v>3</v>
-      </c>
-      <c r="R2" s="7">
+      <c r="V2">
+        <v>3</v>
+      </c>
+      <c r="W2" s="7">
         <f ca="1">TODAY()-L2</f>
         <v>1107</v>
       </c>
-      <c r="S2" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -1279,13 +1366,13 @@
         <v>1200</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>5000</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>1202</v>
@@ -1308,30 +1395,47 @@
       <c r="L3" s="5">
         <v>43393</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="7">
+        <f t="shared" ref="M3:M31" si="0">MONTH(L3)</f>
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>1000</v>
+      </c>
+      <c r="R3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" t="s">
         <v>18</v>
       </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3">
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T31" si="1">LEFT(S3,2)</f>
+        <v>ZW</v>
+      </c>
+      <c r="U3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <v>3</v>
-      </c>
-      <c r="R3" s="7">
-        <f t="shared" ref="R3:R31" ca="1" si="0">TODAY()-L3</f>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3" s="7">
+        <f t="shared" ref="W3:W31" ca="1" si="2">TODAY()-L3</f>
         <v>1107</v>
       </c>
-      <c r="T3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -1339,13 +1443,13 @@
         <v>1300</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>5000</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>1301</v>
@@ -1368,30 +1472,47 @@
       <c r="L4" s="5">
         <v>43393</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>1000</v>
+      </c>
+      <c r="R4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4">
+      <c r="T4" t="str">
+        <f t="shared" si="1"/>
+        <v>ZW</v>
+      </c>
+      <c r="U4">
         <v>1</v>
       </c>
-      <c r="Q4">
-        <v>3</v>
-      </c>
-      <c r="R4" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1107</v>
       </c>
-      <c r="T4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -1399,13 +1520,13 @@
         <v>1300</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>5000</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>1302</v>
@@ -1428,27 +1549,44 @@
       <c r="L5" s="5">
         <v>43393</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>1000</v>
+      </c>
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" t="s">
         <v>18</v>
       </c>
-      <c r="N5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5">
+      <c r="T5" t="str">
+        <f t="shared" si="1"/>
+        <v>ZW</v>
+      </c>
+      <c r="U5">
         <v>1</v>
       </c>
-      <c r="Q5">
-        <v>3</v>
-      </c>
-      <c r="R5" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1107</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1001</v>
       </c>
@@ -1456,13 +1594,13 @@
         <v>1400</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>5100</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <v>1401</v>
@@ -1485,27 +1623,44 @@
       <c r="L6" s="5">
         <v>43391</v>
       </c>
-      <c r="M6" t="s">
-        <v>24</v>
+      <c r="M6" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="O6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6">
+        <v>70</v>
+      </c>
+      <c r="P6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>1001</v>
+      </c>
+      <c r="R6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="1"/>
+        <v>AB</v>
+      </c>
+      <c r="U6">
         <v>0</v>
       </c>
-      <c r="Q6">
-        <v>3</v>
-      </c>
-      <c r="R6" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1109</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1001</v>
       </c>
@@ -1513,13 +1668,13 @@
         <v>1400</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>5100</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7">
         <v>1402</v>
@@ -1542,27 +1697,44 @@
       <c r="L7" s="5">
         <v>43391</v>
       </c>
-      <c r="M7" t="s">
-        <v>24</v>
+      <c r="M7" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="O7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7">
+        <v>70</v>
+      </c>
+      <c r="P7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>1001</v>
+      </c>
+      <c r="R7" t="s">
+        <v>22</v>
+      </c>
+      <c r="S7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="1"/>
+        <v>AB</v>
+      </c>
+      <c r="U7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>3</v>
-      </c>
-      <c r="R7" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1109</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1001</v>
       </c>
@@ -1570,13 +1742,13 @@
         <v>1500</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>5100</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>1501</v>
@@ -1599,27 +1771,44 @@
       <c r="L8" s="5">
         <v>43391</v>
       </c>
-      <c r="M8" t="s">
-        <v>24</v>
+      <c r="M8" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="O8" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8">
+        <v>70</v>
+      </c>
+      <c r="P8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>1001</v>
+      </c>
+      <c r="R8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="1"/>
+        <v>AB</v>
+      </c>
+      <c r="U8">
         <v>0</v>
       </c>
-      <c r="Q8">
-        <v>3</v>
-      </c>
-      <c r="R8" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V8">
+        <v>3</v>
+      </c>
+      <c r="W8" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1109</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1001</v>
       </c>
@@ -1627,13 +1816,13 @@
         <v>1500</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>5100</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>1502</v>
@@ -1656,27 +1845,44 @@
       <c r="L9" s="5">
         <v>43391</v>
       </c>
-      <c r="M9" t="s">
-        <v>24</v>
+      <c r="M9" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="O9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9">
+        <v>70</v>
+      </c>
+      <c r="P9" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>1001</v>
+      </c>
+      <c r="R9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S9" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="1"/>
+        <v>AB</v>
+      </c>
+      <c r="U9">
         <v>0</v>
       </c>
-      <c r="Q9">
-        <v>3</v>
-      </c>
-      <c r="R9" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V9">
+        <v>3</v>
+      </c>
+      <c r="W9" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1109</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1002</v>
       </c>
@@ -1684,13 +1890,13 @@
         <v>1600</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>5100</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10">
         <v>1601</v>
@@ -1713,27 +1919,44 @@
       <c r="L10" s="5">
         <v>43390</v>
       </c>
-      <c r="M10" t="s">
-        <v>29</v>
+      <c r="M10" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N10" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="O10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P10">
+        <v>72</v>
+      </c>
+      <c r="P10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>1002</v>
+      </c>
+      <c r="R10" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="1"/>
+        <v>CD</v>
+      </c>
+      <c r="U10">
         <v>1</v>
       </c>
-      <c r="Q10">
-        <v>3</v>
-      </c>
-      <c r="R10" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V10">
+        <v>3</v>
+      </c>
+      <c r="W10" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1110</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1002</v>
       </c>
@@ -1741,13 +1964,13 @@
         <v>1600</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>5100</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11">
         <v>1602</v>
@@ -1770,27 +1993,44 @@
       <c r="L11" s="5">
         <v>43390</v>
       </c>
-      <c r="M11" t="s">
-        <v>29</v>
+      <c r="M11" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N11" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="O11" t="s">
-        <v>31</v>
-      </c>
-      <c r="P11">
+        <v>72</v>
+      </c>
+      <c r="P11" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>1002</v>
+      </c>
+      <c r="R11" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="1"/>
+        <v>CD</v>
+      </c>
+      <c r="U11">
         <v>1</v>
       </c>
-      <c r="Q11">
-        <v>3</v>
-      </c>
-      <c r="R11" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V11">
+        <v>3</v>
+      </c>
+      <c r="W11" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1110</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1002</v>
       </c>
@@ -1798,13 +2038,13 @@
         <v>1700</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>5200</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F12">
         <v>1701</v>
@@ -1827,27 +2067,44 @@
       <c r="L12" s="5">
         <v>43390</v>
       </c>
-      <c r="M12" t="s">
-        <v>29</v>
+      <c r="M12" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N12" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="O12" t="s">
-        <v>31</v>
-      </c>
-      <c r="P12">
+        <v>72</v>
+      </c>
+      <c r="P12" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>1002</v>
+      </c>
+      <c r="R12" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="1"/>
+        <v>CD</v>
+      </c>
+      <c r="U12">
         <v>1</v>
       </c>
-      <c r="Q12">
-        <v>3</v>
-      </c>
-      <c r="R12" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V12">
+        <v>3</v>
+      </c>
+      <c r="W12" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1110</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1002</v>
       </c>
@@ -1855,13 +2112,13 @@
         <v>1700</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>5200</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F13">
         <v>1702</v>
@@ -1884,27 +2141,44 @@
       <c r="L13" s="5">
         <v>43390</v>
       </c>
-      <c r="M13" t="s">
-        <v>29</v>
+      <c r="M13" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N13" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="O13" t="s">
-        <v>31</v>
-      </c>
-      <c r="P13">
+        <v>72</v>
+      </c>
+      <c r="P13" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>1002</v>
+      </c>
+      <c r="R13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" si="1"/>
+        <v>CD</v>
+      </c>
+      <c r="U13">
         <v>1</v>
       </c>
-      <c r="Q13">
-        <v>3</v>
-      </c>
-      <c r="R13" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V13">
+        <v>3</v>
+      </c>
+      <c r="W13" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1110</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1003</v>
       </c>
@@ -1912,13 +2186,13 @@
         <v>1800</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>5200</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F14">
         <v>1801</v>
@@ -1941,27 +2215,44 @@
       <c r="L14" s="5">
         <v>43388</v>
       </c>
-      <c r="M14" t="s">
-        <v>35</v>
+      <c r="M14" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N14" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="O14" t="s">
-        <v>37</v>
-      </c>
-      <c r="P14">
+        <v>74</v>
+      </c>
+      <c r="P14" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>1003</v>
+      </c>
+      <c r="R14" t="s">
+        <v>31</v>
+      </c>
+      <c r="S14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="1"/>
+        <v>KB</v>
+      </c>
+      <c r="U14">
         <v>0</v>
       </c>
-      <c r="Q14">
-        <v>3</v>
-      </c>
-      <c r="R14" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V14">
+        <v>3</v>
+      </c>
+      <c r="W14" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1112</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1003</v>
       </c>
@@ -1969,13 +2260,13 @@
         <v>1800</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>5200</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F15">
         <v>1802</v>
@@ -1998,27 +2289,44 @@
       <c r="L15" s="5">
         <v>43388</v>
       </c>
-      <c r="M15" t="s">
-        <v>35</v>
+      <c r="M15" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N15" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="O15" t="s">
-        <v>37</v>
-      </c>
-      <c r="P15">
+        <v>74</v>
+      </c>
+      <c r="P15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>1003</v>
+      </c>
+      <c r="R15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S15" t="s">
+        <v>32</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="1"/>
+        <v>KB</v>
+      </c>
+      <c r="U15">
         <v>0</v>
       </c>
-      <c r="Q15">
-        <v>3</v>
-      </c>
-      <c r="R15" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V15">
+        <v>3</v>
+      </c>
+      <c r="W15" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1112</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1003</v>
       </c>
@@ -2026,13 +2334,13 @@
         <v>1900</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>5300</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F16">
         <v>1901</v>
@@ -2055,27 +2363,44 @@
       <c r="L16" s="5">
         <v>43388</v>
       </c>
-      <c r="M16" t="s">
-        <v>35</v>
+      <c r="M16" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N16" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="O16" t="s">
-        <v>37</v>
-      </c>
-      <c r="P16">
+        <v>74</v>
+      </c>
+      <c r="P16" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>1003</v>
+      </c>
+      <c r="R16" t="s">
+        <v>31</v>
+      </c>
+      <c r="S16" t="s">
+        <v>32</v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" si="1"/>
+        <v>KB</v>
+      </c>
+      <c r="U16">
         <v>0</v>
       </c>
-      <c r="Q16">
-        <v>3</v>
-      </c>
-      <c r="R16" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V16">
+        <v>3</v>
+      </c>
+      <c r="W16" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1112</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1003</v>
       </c>
@@ -2083,13 +2408,13 @@
         <v>1900</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D17">
         <v>5300</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F17">
         <v>1902</v>
@@ -2112,27 +2437,44 @@
       <c r="L17" s="5">
         <v>43388</v>
       </c>
-      <c r="M17" t="s">
-        <v>35</v>
+      <c r="M17" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N17" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="O17" t="s">
-        <v>37</v>
-      </c>
-      <c r="P17">
+        <v>74</v>
+      </c>
+      <c r="P17" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>1003</v>
+      </c>
+      <c r="R17" t="s">
+        <v>31</v>
+      </c>
+      <c r="S17" t="s">
+        <v>32</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" si="1"/>
+        <v>KB</v>
+      </c>
+      <c r="U17">
         <v>0</v>
       </c>
-      <c r="Q17">
-        <v>3</v>
-      </c>
-      <c r="R17" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V17">
+        <v>3</v>
+      </c>
+      <c r="W17" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1112</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1004</v>
       </c>
@@ -2140,13 +2482,13 @@
         <v>2000</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D18">
         <v>5300</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F18">
         <v>2001</v>
@@ -2169,27 +2511,44 @@
       <c r="L18" s="5">
         <v>43392</v>
       </c>
-      <c r="M18" t="s">
-        <v>41</v>
+      <c r="M18" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N18" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="O18" t="s">
-        <v>43</v>
-      </c>
-      <c r="P18">
+        <v>76</v>
+      </c>
+      <c r="P18" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>1004</v>
+      </c>
+      <c r="R18" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" t="s">
+        <v>37</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="1"/>
+        <v>IK</v>
+      </c>
+      <c r="U18">
         <v>1</v>
       </c>
-      <c r="Q18">
-        <v>3</v>
-      </c>
-      <c r="R18" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V18">
+        <v>3</v>
+      </c>
+      <c r="W18" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1108</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1004</v>
       </c>
@@ -2197,13 +2556,13 @@
         <v>2000</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>5300</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F19">
         <v>2002</v>
@@ -2226,27 +2585,44 @@
       <c r="L19" s="5">
         <v>43392</v>
       </c>
-      <c r="M19" t="s">
-        <v>41</v>
+      <c r="M19" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N19" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="O19" t="s">
-        <v>43</v>
-      </c>
-      <c r="P19">
+        <v>76</v>
+      </c>
+      <c r="P19" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>1004</v>
+      </c>
+      <c r="R19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="1"/>
+        <v>IK</v>
+      </c>
+      <c r="U19">
         <v>1</v>
       </c>
-      <c r="Q19">
-        <v>3</v>
-      </c>
-      <c r="R19" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V19">
+        <v>3</v>
+      </c>
+      <c r="W19" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1108</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1004</v>
       </c>
@@ -2254,13 +2630,13 @@
         <v>2100</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>5400</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F20">
         <v>2101</v>
@@ -2283,27 +2659,44 @@
       <c r="L20" s="5">
         <v>43392</v>
       </c>
-      <c r="M20" t="s">
-        <v>41</v>
+      <c r="M20" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N20" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="O20" t="s">
-        <v>43</v>
-      </c>
-      <c r="P20">
+        <v>76</v>
+      </c>
+      <c r="P20" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>1004</v>
+      </c>
+      <c r="R20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S20" t="s">
+        <v>37</v>
+      </c>
+      <c r="T20" t="str">
+        <f t="shared" si="1"/>
+        <v>IK</v>
+      </c>
+      <c r="U20">
         <v>1</v>
       </c>
-      <c r="Q20">
-        <v>3</v>
-      </c>
-      <c r="R20" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V20">
+        <v>3</v>
+      </c>
+      <c r="W20" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1108</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1004</v>
       </c>
@@ -2311,13 +2704,13 @@
         <v>2100</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>5400</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F21">
         <v>2102</v>
@@ -2340,27 +2733,44 @@
       <c r="L21" s="5">
         <v>43392</v>
       </c>
-      <c r="M21" t="s">
-        <v>41</v>
+      <c r="M21" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N21" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="O21" t="s">
-        <v>43</v>
-      </c>
-      <c r="P21">
+        <v>76</v>
+      </c>
+      <c r="P21" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>1004</v>
+      </c>
+      <c r="R21" t="s">
+        <v>36</v>
+      </c>
+      <c r="S21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T21" t="str">
+        <f t="shared" si="1"/>
+        <v>IK</v>
+      </c>
+      <c r="U21">
         <v>1</v>
       </c>
-      <c r="Q21">
-        <v>3</v>
-      </c>
-      <c r="R21" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V21">
+        <v>3</v>
+      </c>
+      <c r="W21" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1108</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1004</v>
       </c>
@@ -2368,13 +2778,13 @@
         <v>2200</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D22">
         <v>5400</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F22">
         <v>2201</v>
@@ -2397,27 +2807,44 @@
       <c r="L22" s="5">
         <v>43392</v>
       </c>
-      <c r="M22" t="s">
-        <v>41</v>
+      <c r="M22" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N22" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="O22" t="s">
-        <v>43</v>
-      </c>
-      <c r="P22">
+        <v>76</v>
+      </c>
+      <c r="P22" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>1004</v>
+      </c>
+      <c r="R22" t="s">
+        <v>36</v>
+      </c>
+      <c r="S22" t="s">
+        <v>37</v>
+      </c>
+      <c r="T22" t="str">
+        <f t="shared" si="1"/>
+        <v>IK</v>
+      </c>
+      <c r="U22">
         <v>1</v>
       </c>
-      <c r="Q22">
-        <v>3</v>
-      </c>
-      <c r="R22" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V22">
+        <v>3</v>
+      </c>
+      <c r="W22" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1108</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1004</v>
       </c>
@@ -2425,13 +2852,13 @@
         <v>2200</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>5400</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F23">
         <v>2202</v>
@@ -2454,27 +2881,44 @@
       <c r="L23" s="5">
         <v>43392</v>
       </c>
-      <c r="M23" t="s">
-        <v>41</v>
+      <c r="M23" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N23" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="O23" t="s">
-        <v>43</v>
-      </c>
-      <c r="P23">
+        <v>76</v>
+      </c>
+      <c r="P23" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>1004</v>
+      </c>
+      <c r="R23" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" t="s">
+        <v>37</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="1"/>
+        <v>IK</v>
+      </c>
+      <c r="U23">
         <v>1</v>
       </c>
-      <c r="Q23">
-        <v>3</v>
-      </c>
-      <c r="R23" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V23">
+        <v>3</v>
+      </c>
+      <c r="W23" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1108</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1005</v>
       </c>
@@ -2482,13 +2926,13 @@
         <v>2300</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D24">
         <v>5500</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F24">
         <v>2301</v>
@@ -2511,27 +2955,44 @@
       <c r="L24" s="5">
         <v>43389</v>
       </c>
-      <c r="M24" t="s">
-        <v>49</v>
+      <c r="M24" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N24" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="O24" t="s">
-        <v>51</v>
-      </c>
-      <c r="P24">
+        <v>78</v>
+      </c>
+      <c r="P24" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>1005</v>
+      </c>
+      <c r="R24" t="s">
+        <v>43</v>
+      </c>
+      <c r="S24" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24" t="str">
+        <f t="shared" si="1"/>
+        <v>OP</v>
+      </c>
+      <c r="U24">
         <v>0</v>
       </c>
-      <c r="Q24">
-        <v>3</v>
-      </c>
-      <c r="R24" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V24">
+        <v>3</v>
+      </c>
+      <c r="W24" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1111</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1005</v>
       </c>
@@ -2539,13 +3000,13 @@
         <v>2300</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D25">
         <v>5500</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F25">
         <v>2302</v>
@@ -2568,27 +3029,44 @@
       <c r="L25" s="5">
         <v>43389</v>
       </c>
-      <c r="M25" t="s">
-        <v>49</v>
+      <c r="M25" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N25" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="O25" t="s">
-        <v>51</v>
-      </c>
-      <c r="P25">
+        <v>78</v>
+      </c>
+      <c r="P25" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>1005</v>
+      </c>
+      <c r="R25" t="s">
+        <v>43</v>
+      </c>
+      <c r="S25" t="s">
+        <v>44</v>
+      </c>
+      <c r="T25" t="str">
+        <f t="shared" si="1"/>
+        <v>OP</v>
+      </c>
+      <c r="U25">
         <v>0</v>
       </c>
-      <c r="Q25">
-        <v>3</v>
-      </c>
-      <c r="R25" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V25">
+        <v>3</v>
+      </c>
+      <c r="W25" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1111</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1005</v>
       </c>
@@ -2596,13 +3074,13 @@
         <v>2400</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D26">
         <v>5500</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F26">
         <v>2401</v>
@@ -2625,27 +3103,44 @@
       <c r="L26" s="5">
         <v>43389</v>
       </c>
-      <c r="M26" t="s">
-        <v>49</v>
+      <c r="M26" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N26" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="O26" t="s">
-        <v>51</v>
-      </c>
-      <c r="P26">
+        <v>78</v>
+      </c>
+      <c r="P26" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>1005</v>
+      </c>
+      <c r="R26" t="s">
+        <v>43</v>
+      </c>
+      <c r="S26" t="s">
+        <v>44</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="1"/>
+        <v>OP</v>
+      </c>
+      <c r="U26">
         <v>0</v>
       </c>
-      <c r="Q26">
-        <v>3</v>
-      </c>
-      <c r="R26" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V26">
+        <v>3</v>
+      </c>
+      <c r="W26" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1111</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1006</v>
       </c>
@@ -2653,13 +3148,13 @@
         <v>2400</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D27">
         <v>5500</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F27">
         <v>2402</v>
@@ -2682,27 +3177,44 @@
       <c r="L27" s="5">
         <v>43397</v>
       </c>
-      <c r="M27" t="s">
-        <v>53</v>
+      <c r="M27" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N27" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="O27" t="s">
-        <v>55</v>
-      </c>
-      <c r="P27">
+        <v>80</v>
+      </c>
+      <c r="P27" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>1006</v>
+      </c>
+      <c r="R27" t="s">
+        <v>46</v>
+      </c>
+      <c r="S27" t="s">
+        <v>47</v>
+      </c>
+      <c r="T27" t="str">
+        <f t="shared" si="1"/>
+        <v>XH</v>
+      </c>
+      <c r="U27">
         <v>1</v>
       </c>
-      <c r="Q27">
-        <v>3</v>
-      </c>
-      <c r="R27" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V27">
+        <v>3</v>
+      </c>
+      <c r="W27" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1103</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1006</v>
       </c>
@@ -2710,13 +3222,13 @@
         <v>2500</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D28">
         <v>5600</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F28">
         <v>2501</v>
@@ -2739,27 +3251,44 @@
       <c r="L28" s="5">
         <v>43397</v>
       </c>
-      <c r="M28" t="s">
-        <v>53</v>
+      <c r="M28" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N28" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="O28" t="s">
-        <v>55</v>
-      </c>
-      <c r="P28">
+        <v>80</v>
+      </c>
+      <c r="P28" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>1006</v>
+      </c>
+      <c r="R28" t="s">
+        <v>46</v>
+      </c>
+      <c r="S28" t="s">
+        <v>47</v>
+      </c>
+      <c r="T28" t="str">
+        <f t="shared" si="1"/>
+        <v>XH</v>
+      </c>
+      <c r="U28">
         <v>1</v>
       </c>
-      <c r="Q28">
-        <v>3</v>
-      </c>
-      <c r="R28" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V28">
+        <v>3</v>
+      </c>
+      <c r="W28" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1103</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1006</v>
       </c>
@@ -2767,13 +3296,13 @@
         <v>2500</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D29">
         <v>5600</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F29">
         <v>2502</v>
@@ -2796,27 +3325,44 @@
       <c r="L29" s="5">
         <v>43397</v>
       </c>
-      <c r="M29" t="s">
-        <v>53</v>
+      <c r="M29" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N29" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="O29" t="s">
-        <v>55</v>
-      </c>
-      <c r="P29">
+        <v>80</v>
+      </c>
+      <c r="P29" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>1006</v>
+      </c>
+      <c r="R29" t="s">
+        <v>46</v>
+      </c>
+      <c r="S29" t="s">
+        <v>47</v>
+      </c>
+      <c r="T29" t="str">
+        <f t="shared" si="1"/>
+        <v>XH</v>
+      </c>
+      <c r="U29">
         <v>1</v>
       </c>
-      <c r="Q29">
-        <v>3</v>
-      </c>
-      <c r="R29" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V29">
+        <v>3</v>
+      </c>
+      <c r="W29" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1103</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1006</v>
       </c>
@@ -2824,13 +3370,13 @@
         <v>2600</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D30">
         <v>5600</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F30">
         <v>2601</v>
@@ -2853,27 +3399,44 @@
       <c r="L30" s="5">
         <v>43397</v>
       </c>
-      <c r="M30" t="s">
-        <v>53</v>
+      <c r="M30" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N30" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="O30" t="s">
-        <v>55</v>
-      </c>
-      <c r="P30">
+        <v>80</v>
+      </c>
+      <c r="P30" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>1006</v>
+      </c>
+      <c r="R30" t="s">
+        <v>46</v>
+      </c>
+      <c r="S30" t="s">
+        <v>47</v>
+      </c>
+      <c r="T30" t="str">
+        <f t="shared" si="1"/>
+        <v>XH</v>
+      </c>
+      <c r="U30">
         <v>1</v>
       </c>
-      <c r="Q30">
-        <v>3</v>
-      </c>
-      <c r="R30" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V30">
+        <v>3</v>
+      </c>
+      <c r="W30" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1103</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1006</v>
       </c>
@@ -2881,13 +3444,13 @@
         <v>2600</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D31">
         <v>5600</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F31">
         <v>2602</v>
@@ -2910,30 +3473,47 @@
       <c r="L31" s="5">
         <v>43397</v>
       </c>
-      <c r="M31" t="s">
-        <v>53</v>
+      <c r="M31" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="N31" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="O31" t="s">
-        <v>55</v>
-      </c>
-      <c r="P31">
+        <v>80</v>
+      </c>
+      <c r="P31" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>1006</v>
+      </c>
+      <c r="R31" t="s">
+        <v>46</v>
+      </c>
+      <c r="S31" t="s">
+        <v>47</v>
+      </c>
+      <c r="T31" t="str">
+        <f t="shared" si="1"/>
+        <v>XH</v>
+      </c>
+      <c r="U31">
         <v>1</v>
       </c>
-      <c r="Q31">
-        <v>3</v>
-      </c>
-      <c r="R31" s="7">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V31">
+        <v>3</v>
+      </c>
+      <c r="W31" s="7">
+        <f t="shared" ca="1" si="2"/>
         <v>1103</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T4 T8">
-      <formula1>INDIRECT( $S2)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y4 Y8">
+      <formula1>INDIRECT( $X2)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2945,7 +3525,7 @@
           <x14:formula1>
             <xm:f>Hoja1!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>S2</xm:sqref>
+          <xm:sqref>X2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2965,67 +3545,67 @@
   <sheetData>
     <row r="1" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>